<commit_message>
actualizacion de modelo entidad-relacion
</commit_message>
<xml_diff>
--- a/analisis de tablas.xlsx
+++ b/analisis de tablas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell E6420\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rony Vidaur\Desktop\Jocs\Bases\proyecto\repo\Proyecto-BD\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -688,7 +688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:X43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K8" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G19" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
       <selection activeCell="P41" sqref="P41"/>
     </sheetView>
   </sheetViews>

</xml_diff>